<commit_message>
Edit Income Codes for report
</commit_message>
<xml_diff>
--- a/R/FractioninData.xlsx
+++ b/R/FractioninData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FractioninData" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="15">
   <si>
     <t>Percentile</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t>Minus</t>
+  </si>
+  <si>
+    <t>before</t>
+  </si>
+  <si>
+    <t>after</t>
+  </si>
+  <si>
+    <t>V1</t>
   </si>
 </sst>
 </file>
@@ -404,7 +413,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -539,6 +548,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD6DADC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD6DADC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD6DADC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD6DADC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD6DADC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -584,7 +617,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -605,6 +638,15 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -8772,10 +8814,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I33"/>
+  <dimension ref="A2:I209"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:I2"/>
+    <sheetView tabSelected="1" topLeftCell="A198" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H209" sqref="H179:I209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9703,7 +9745,4151 @@
         <v>78.635802400000003</v>
       </c>
     </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G34" s="8">
+        <f t="shared" ref="G34:G69" si="4">C34*100</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="8">
+        <f t="shared" ref="H34:H69" si="5">D34*100</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="8">
+        <f t="shared" ref="I34:I69" si="6">E34*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G35" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H35" s="8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I35" s="8">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
+      <c r="C36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="8" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H36" s="8" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I36" s="8">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="G37" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H37" s="8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I37" s="8">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="G38" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H38" s="8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I38" s="8">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="6">
+        <v>1</v>
+      </c>
+      <c r="C39" s="7">
+        <v>0</v>
+      </c>
+      <c r="D39" s="7">
+        <v>0.27719779999999999</v>
+      </c>
+      <c r="E39" s="7">
+        <v>0.2703837</v>
+      </c>
+      <c r="G39" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H39" s="8">
+        <f t="shared" si="5"/>
+        <v>27.71978</v>
+      </c>
+      <c r="I39" s="8">
+        <f t="shared" si="6"/>
+        <v>27.03837</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="6">
+        <v>2</v>
+      </c>
+      <c r="C40" s="7">
+        <v>1</v>
+      </c>
+      <c r="D40" s="7">
+        <v>0.30081612000000002</v>
+      </c>
+      <c r="E40" s="7">
+        <v>0.62391529999999995</v>
+      </c>
+      <c r="G40" s="8">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="H40" s="8">
+        <f t="shared" si="5"/>
+        <v>30.081612000000003</v>
+      </c>
+      <c r="I40" s="8">
+        <f t="shared" si="6"/>
+        <v>62.391529999999996</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="6">
+        <v>3</v>
+      </c>
+      <c r="C41" s="7">
+        <v>2</v>
+      </c>
+      <c r="D41" s="7">
+        <v>0.35742241000000002</v>
+      </c>
+      <c r="E41" s="7">
+        <v>0.78894010000000003</v>
+      </c>
+      <c r="G41" s="8">
+        <f t="shared" si="4"/>
+        <v>200</v>
+      </c>
+      <c r="H41" s="8">
+        <f t="shared" si="5"/>
+        <v>35.742241</v>
+      </c>
+      <c r="I41" s="8">
+        <f t="shared" si="6"/>
+        <v>78.894010000000009</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="6">
+        <v>4</v>
+      </c>
+      <c r="C42" s="7">
+        <v>3</v>
+      </c>
+      <c r="D42" s="7">
+        <v>0.25639138</v>
+      </c>
+      <c r="E42" s="7">
+        <v>0.37315890000000002</v>
+      </c>
+      <c r="G42" s="8">
+        <f t="shared" si="4"/>
+        <v>300</v>
+      </c>
+      <c r="H42" s="8">
+        <f t="shared" si="5"/>
+        <v>25.639137999999999</v>
+      </c>
+      <c r="I42" s="8">
+        <f t="shared" si="6"/>
+        <v>37.315890000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="6">
+        <v>5</v>
+      </c>
+      <c r="C43" s="7">
+        <v>4</v>
+      </c>
+      <c r="D43" s="7">
+        <v>0.21609117999999999</v>
+      </c>
+      <c r="E43" s="7">
+        <v>0.32213190000000003</v>
+      </c>
+      <c r="G43" s="8">
+        <f t="shared" si="4"/>
+        <v>400</v>
+      </c>
+      <c r="H43" s="8">
+        <f t="shared" si="5"/>
+        <v>21.609117999999999</v>
+      </c>
+      <c r="I43" s="8">
+        <f t="shared" si="6"/>
+        <v>32.213190000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="6">
+        <v>6</v>
+      </c>
+      <c r="C44" s="7">
+        <v>5</v>
+      </c>
+      <c r="D44" s="7">
+        <v>0.30281807999999999</v>
+      </c>
+      <c r="E44" s="7">
+        <v>0.46033669999999999</v>
+      </c>
+      <c r="G44" s="8">
+        <f t="shared" si="4"/>
+        <v>500</v>
+      </c>
+      <c r="H44" s="8">
+        <f t="shared" si="5"/>
+        <v>30.281807999999998</v>
+      </c>
+      <c r="I44" s="8">
+        <f t="shared" si="6"/>
+        <v>46.033670000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="6">
+        <v>7</v>
+      </c>
+      <c r="C45" s="7">
+        <v>6</v>
+      </c>
+      <c r="D45" s="7">
+        <v>0.25910369</v>
+      </c>
+      <c r="E45" s="7">
+        <v>0.2720397</v>
+      </c>
+      <c r="G45" s="8">
+        <f t="shared" si="4"/>
+        <v>600</v>
+      </c>
+      <c r="H45" s="8">
+        <f t="shared" si="5"/>
+        <v>25.910368999999999</v>
+      </c>
+      <c r="I45" s="8">
+        <f t="shared" si="6"/>
+        <v>27.203969999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="6">
+        <v>8</v>
+      </c>
+      <c r="C46" s="7">
+        <v>7</v>
+      </c>
+      <c r="D46" s="7">
+        <v>0.32310016000000003</v>
+      </c>
+      <c r="E46" s="7">
+        <v>0.30584119999999998</v>
+      </c>
+      <c r="G46" s="8">
+        <f t="shared" si="4"/>
+        <v>700</v>
+      </c>
+      <c r="H46" s="8">
+        <f t="shared" si="5"/>
+        <v>32.310016000000005</v>
+      </c>
+      <c r="I46" s="8">
+        <f t="shared" si="6"/>
+        <v>30.584119999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="6">
+        <v>9</v>
+      </c>
+      <c r="C47" s="7">
+        <v>8</v>
+      </c>
+      <c r="D47" s="7">
+        <v>0.10287505</v>
+      </c>
+      <c r="E47" s="7">
+        <v>0.1080236</v>
+      </c>
+      <c r="G47" s="8">
+        <f t="shared" si="4"/>
+        <v>800</v>
+      </c>
+      <c r="H47" s="8">
+        <f t="shared" si="5"/>
+        <v>10.287504999999999</v>
+      </c>
+      <c r="I47" s="8">
+        <f t="shared" si="6"/>
+        <v>10.80236</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="6">
+        <v>10</v>
+      </c>
+      <c r="C48" s="7">
+        <v>9</v>
+      </c>
+      <c r="D48" s="7">
+        <v>0.30309725999999998</v>
+      </c>
+      <c r="E48" s="7">
+        <v>0.39816040000000003</v>
+      </c>
+      <c r="G48" s="8">
+        <f t="shared" si="4"/>
+        <v>900</v>
+      </c>
+      <c r="H48" s="8">
+        <f t="shared" si="5"/>
+        <v>30.309725999999998</v>
+      </c>
+      <c r="I48" s="8">
+        <f t="shared" si="6"/>
+        <v>39.816040000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="6">
+        <v>11</v>
+      </c>
+      <c r="C49" s="7">
+        <v>10</v>
+      </c>
+      <c r="D49" s="7">
+        <v>0.34671271999999997</v>
+      </c>
+      <c r="E49" s="7">
+        <v>0.37637579999999998</v>
+      </c>
+      <c r="G49" s="8">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="H49" s="8">
+        <f t="shared" si="5"/>
+        <v>34.671271999999995</v>
+      </c>
+      <c r="I49" s="8">
+        <f t="shared" si="6"/>
+        <v>37.63758</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="6">
+        <v>12</v>
+      </c>
+      <c r="C50" s="7">
+        <v>11</v>
+      </c>
+      <c r="D50" s="7">
+        <v>8.3133390000000001E-2</v>
+      </c>
+      <c r="E50" s="7">
+        <v>0.1330287</v>
+      </c>
+      <c r="G50" s="8">
+        <f t="shared" si="4"/>
+        <v>1100</v>
+      </c>
+      <c r="H50" s="8">
+        <f t="shared" si="5"/>
+        <v>8.3133390000000009</v>
+      </c>
+      <c r="I50" s="8">
+        <f t="shared" si="6"/>
+        <v>13.30287</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="6">
+        <v>13</v>
+      </c>
+      <c r="C51" s="7">
+        <v>12</v>
+      </c>
+      <c r="D51" s="7">
+        <v>0.21779019999999999</v>
+      </c>
+      <c r="E51" s="7">
+        <v>0.2429856</v>
+      </c>
+      <c r="G51" s="8">
+        <f t="shared" si="4"/>
+        <v>1200</v>
+      </c>
+      <c r="H51" s="8">
+        <f t="shared" si="5"/>
+        <v>21.779019999999999</v>
+      </c>
+      <c r="I51" s="8">
+        <f t="shared" si="6"/>
+        <v>24.298559999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="6">
+        <v>14</v>
+      </c>
+      <c r="C52" s="7">
+        <v>13</v>
+      </c>
+      <c r="D52" s="7">
+        <v>0.24836196999999999</v>
+      </c>
+      <c r="E52" s="7">
+        <v>0.46498099999999998</v>
+      </c>
+      <c r="G52" s="8">
+        <f t="shared" si="4"/>
+        <v>1300</v>
+      </c>
+      <c r="H52" s="8">
+        <f t="shared" si="5"/>
+        <v>24.836196999999999</v>
+      </c>
+      <c r="I52" s="8">
+        <f t="shared" si="6"/>
+        <v>46.498100000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="6">
+        <v>15</v>
+      </c>
+      <c r="C53" s="7">
+        <v>14</v>
+      </c>
+      <c r="D53" s="7">
+        <v>0.26394053000000001</v>
+      </c>
+      <c r="E53" s="7">
+        <v>0.14955950000000001</v>
+      </c>
+      <c r="G53" s="8">
+        <f t="shared" si="4"/>
+        <v>1400</v>
+      </c>
+      <c r="H53" s="8">
+        <f t="shared" si="5"/>
+        <v>26.394053</v>
+      </c>
+      <c r="I53" s="8">
+        <f t="shared" si="6"/>
+        <v>14.955950000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="6">
+        <v>16</v>
+      </c>
+      <c r="C54" s="7">
+        <v>15</v>
+      </c>
+      <c r="D54" s="7">
+        <v>0.15963390999999999</v>
+      </c>
+      <c r="E54" s="7">
+        <v>0.36065849999999999</v>
+      </c>
+      <c r="G54" s="8">
+        <f t="shared" si="4"/>
+        <v>1500</v>
+      </c>
+      <c r="H54" s="8">
+        <f t="shared" si="5"/>
+        <v>15.963391</v>
+      </c>
+      <c r="I54" s="8">
+        <f t="shared" si="6"/>
+        <v>36.065849999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="6">
+        <v>17</v>
+      </c>
+      <c r="C55" s="7">
+        <v>16</v>
+      </c>
+      <c r="D55" s="7">
+        <v>0.15416198</v>
+      </c>
+      <c r="E55" s="7">
+        <v>0.39329730000000002</v>
+      </c>
+      <c r="G55" s="8">
+        <f t="shared" si="4"/>
+        <v>1600</v>
+      </c>
+      <c r="H55" s="8">
+        <f t="shared" si="5"/>
+        <v>15.416198</v>
+      </c>
+      <c r="I55" s="8">
+        <f t="shared" si="6"/>
+        <v>39.329730000000005</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="6">
+        <v>18</v>
+      </c>
+      <c r="C56" s="7">
+        <v>17</v>
+      </c>
+      <c r="D56" s="7">
+        <v>0.32196269</v>
+      </c>
+      <c r="E56" s="7">
+        <v>0.11587509999999999</v>
+      </c>
+      <c r="G56" s="8">
+        <f t="shared" si="4"/>
+        <v>1700</v>
+      </c>
+      <c r="H56" s="8">
+        <f t="shared" si="5"/>
+        <v>32.196269000000001</v>
+      </c>
+      <c r="I56" s="8">
+        <f t="shared" si="6"/>
+        <v>11.58751</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="6">
+        <v>19</v>
+      </c>
+      <c r="C57" s="7">
+        <v>18</v>
+      </c>
+      <c r="D57" s="7">
+        <v>0.26829756999999999</v>
+      </c>
+      <c r="E57" s="7">
+        <v>0.3413137</v>
+      </c>
+      <c r="G57" s="8">
+        <f t="shared" si="4"/>
+        <v>1800</v>
+      </c>
+      <c r="H57" s="8">
+        <f t="shared" si="5"/>
+        <v>26.829756999999997</v>
+      </c>
+      <c r="I57" s="8">
+        <f t="shared" si="6"/>
+        <v>34.131369999999997</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="6">
+        <v>20</v>
+      </c>
+      <c r="C58" s="7">
+        <v>19</v>
+      </c>
+      <c r="D58" s="7">
+        <v>0.26796398999999999</v>
+      </c>
+      <c r="E58" s="7">
+        <v>0.46400599999999997</v>
+      </c>
+      <c r="G58" s="8">
+        <f t="shared" si="4"/>
+        <v>1900</v>
+      </c>
+      <c r="H58" s="8">
+        <f t="shared" si="5"/>
+        <v>26.796398999999997</v>
+      </c>
+      <c r="I58" s="8">
+        <f t="shared" si="6"/>
+        <v>46.400599999999997</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="6">
+        <v>21</v>
+      </c>
+      <c r="C59" s="7">
+        <v>20</v>
+      </c>
+      <c r="D59" s="7">
+        <v>0.17165685</v>
+      </c>
+      <c r="E59" s="7">
+        <v>0.43221670000000001</v>
+      </c>
+      <c r="G59" s="8">
+        <f t="shared" si="4"/>
+        <v>2000</v>
+      </c>
+      <c r="H59" s="8">
+        <f t="shared" si="5"/>
+        <v>17.165685</v>
+      </c>
+      <c r="I59" s="8">
+        <f t="shared" si="6"/>
+        <v>43.221670000000003</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="6">
+        <v>22</v>
+      </c>
+      <c r="C60" s="7">
+        <v>21</v>
+      </c>
+      <c r="D60" s="7">
+        <v>0.28956977</v>
+      </c>
+      <c r="E60" s="7">
+        <v>0.3623112</v>
+      </c>
+      <c r="G60" s="8">
+        <f t="shared" si="4"/>
+        <v>2100</v>
+      </c>
+      <c r="H60" s="8">
+        <f t="shared" si="5"/>
+        <v>28.956977000000002</v>
+      </c>
+      <c r="I60" s="8">
+        <f t="shared" si="6"/>
+        <v>36.231119999999997</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="6">
+        <v>23</v>
+      </c>
+      <c r="C61" s="7">
+        <v>22</v>
+      </c>
+      <c r="D61" s="7">
+        <v>0.33251364999999999</v>
+      </c>
+      <c r="E61" s="7">
+        <v>0.25707219999999997</v>
+      </c>
+      <c r="G61" s="8">
+        <f t="shared" si="4"/>
+        <v>2200</v>
+      </c>
+      <c r="H61" s="8">
+        <f t="shared" si="5"/>
+        <v>33.251365</v>
+      </c>
+      <c r="I61" s="8">
+        <f t="shared" si="6"/>
+        <v>25.707219999999996</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="6">
+        <v>24</v>
+      </c>
+      <c r="C62" s="7">
+        <v>23</v>
+      </c>
+      <c r="D62" s="7">
+        <v>0.64900698999999995</v>
+      </c>
+      <c r="E62" s="7">
+        <v>0.38320739999999998</v>
+      </c>
+      <c r="G62" s="8">
+        <f t="shared" si="4"/>
+        <v>2300</v>
+      </c>
+      <c r="H62" s="8">
+        <f t="shared" si="5"/>
+        <v>64.900698999999989</v>
+      </c>
+      <c r="I62" s="8">
+        <f t="shared" si="6"/>
+        <v>38.320740000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="6">
+        <v>25</v>
+      </c>
+      <c r="C63" s="7">
+        <v>24</v>
+      </c>
+      <c r="D63" s="7">
+        <v>0.25086930000000002</v>
+      </c>
+      <c r="E63" s="7">
+        <v>0.2349765</v>
+      </c>
+      <c r="G63" s="8">
+        <f t="shared" si="4"/>
+        <v>2400</v>
+      </c>
+      <c r="H63" s="8">
+        <f t="shared" si="5"/>
+        <v>25.086930000000002</v>
+      </c>
+      <c r="I63" s="8">
+        <f t="shared" si="6"/>
+        <v>23.49765</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="6">
+        <v>26</v>
+      </c>
+      <c r="C64" s="7">
+        <v>25</v>
+      </c>
+      <c r="D64" s="7">
+        <v>0.24009860999999999</v>
+      </c>
+      <c r="E64" s="7">
+        <v>0.30037160000000002</v>
+      </c>
+      <c r="G64" s="8">
+        <f t="shared" si="4"/>
+        <v>2500</v>
+      </c>
+      <c r="H64" s="8">
+        <f t="shared" si="5"/>
+        <v>24.009861000000001</v>
+      </c>
+      <c r="I64" s="8">
+        <f t="shared" si="6"/>
+        <v>30.03716</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="6">
+        <v>27</v>
+      </c>
+      <c r="C65" s="7">
+        <v>26</v>
+      </c>
+      <c r="D65" s="7">
+        <v>0.34102914000000001</v>
+      </c>
+      <c r="E65" s="7">
+        <v>0.45293519999999998</v>
+      </c>
+      <c r="G65" s="8">
+        <f t="shared" si="4"/>
+        <v>2600</v>
+      </c>
+      <c r="H65" s="8">
+        <f t="shared" si="5"/>
+        <v>34.102913999999998</v>
+      </c>
+      <c r="I65" s="8">
+        <f t="shared" si="6"/>
+        <v>45.293520000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="6">
+        <v>28</v>
+      </c>
+      <c r="C66" s="7">
+        <v>27</v>
+      </c>
+      <c r="D66" s="7">
+        <v>0.23858592000000001</v>
+      </c>
+      <c r="E66" s="7">
+        <v>0.4475635</v>
+      </c>
+      <c r="G66" s="8">
+        <f t="shared" si="4"/>
+        <v>2700</v>
+      </c>
+      <c r="H66" s="8">
+        <f t="shared" si="5"/>
+        <v>23.858592000000002</v>
+      </c>
+      <c r="I66" s="8">
+        <f t="shared" si="6"/>
+        <v>44.756349999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="6">
+        <v>29</v>
+      </c>
+      <c r="C67" s="7">
+        <v>28</v>
+      </c>
+      <c r="D67" s="7">
+        <v>0.18686116</v>
+      </c>
+      <c r="E67" s="7">
+        <v>0.25097839999999999</v>
+      </c>
+      <c r="G67" s="8">
+        <f t="shared" si="4"/>
+        <v>2800</v>
+      </c>
+      <c r="H67" s="8">
+        <f t="shared" si="5"/>
+        <v>18.686115999999998</v>
+      </c>
+      <c r="I67" s="8">
+        <f t="shared" si="6"/>
+        <v>25.097839999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="6">
+        <v>30</v>
+      </c>
+      <c r="C68" s="7">
+        <v>29</v>
+      </c>
+      <c r="D68" s="7">
+        <v>0.11398968</v>
+      </c>
+      <c r="E68" s="7">
+        <v>0.16749790000000001</v>
+      </c>
+      <c r="G68" s="8">
+        <f t="shared" si="4"/>
+        <v>2900</v>
+      </c>
+      <c r="H68" s="8">
+        <f t="shared" si="5"/>
+        <v>11.398968</v>
+      </c>
+      <c r="I68" s="8">
+        <f t="shared" si="6"/>
+        <v>16.749790000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="6">
+        <v>31</v>
+      </c>
+      <c r="C69" s="7">
+        <v>30</v>
+      </c>
+      <c r="D69" s="7">
+        <v>0.56290934000000004</v>
+      </c>
+      <c r="E69" s="7">
+        <v>0.39238859999999998</v>
+      </c>
+      <c r="G69" s="8">
+        <f t="shared" si="4"/>
+        <v>3000</v>
+      </c>
+      <c r="H69" s="8">
+        <f t="shared" si="5"/>
+        <v>56.290934000000007</v>
+      </c>
+      <c r="I69" s="8">
+        <f t="shared" si="6"/>
+        <v>39.238859999999995</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G70" s="8">
+        <f t="shared" ref="G70:G103" si="7">C70*100</f>
+        <v>0</v>
+      </c>
+      <c r="H70" s="8">
+        <f t="shared" ref="H70:H103" si="8">D70*100</f>
+        <v>0</v>
+      </c>
+      <c r="I70" s="8">
+        <f t="shared" ref="I70:I103" si="9">E70*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C71" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G71" s="8" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H71" s="8" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I71" s="8">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="G72" s="8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H72" s="8">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I72" s="8">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C73" s="6">
+        <v>6</v>
+      </c>
+      <c r="D73" s="7">
+        <v>0</v>
+      </c>
+      <c r="E73" s="7">
+        <v>0.55352769999999996</v>
+      </c>
+      <c r="G73" s="8">
+        <f t="shared" si="7"/>
+        <v>600</v>
+      </c>
+      <c r="H73" s="8">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I73" s="8">
+        <f t="shared" si="9"/>
+        <v>55.352769999999992</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C74" s="6">
+        <v>7</v>
+      </c>
+      <c r="D74" s="7">
+        <v>1</v>
+      </c>
+      <c r="E74" s="7">
+        <v>0.54591250000000002</v>
+      </c>
+      <c r="G74" s="8">
+        <f t="shared" si="7"/>
+        <v>700</v>
+      </c>
+      <c r="H74" s="8">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="I74" s="8">
+        <f t="shared" si="9"/>
+        <v>54.591250000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C75" s="6">
+        <v>8</v>
+      </c>
+      <c r="D75" s="7">
+        <v>2</v>
+      </c>
+      <c r="E75" s="7">
+        <v>0.66652400000000001</v>
+      </c>
+      <c r="G75" s="8">
+        <f t="shared" si="7"/>
+        <v>800</v>
+      </c>
+      <c r="H75" s="8">
+        <f t="shared" si="8"/>
+        <v>200</v>
+      </c>
+      <c r="I75" s="8">
+        <f t="shared" si="9"/>
+        <v>66.6524</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C76" s="6">
+        <v>12</v>
+      </c>
+      <c r="D76" s="7">
+        <v>3</v>
+      </c>
+      <c r="E76" s="7">
+        <v>0.60627379999999997</v>
+      </c>
+      <c r="G76" s="8">
+        <f t="shared" si="7"/>
+        <v>1200</v>
+      </c>
+      <c r="H76" s="8">
+        <f t="shared" si="8"/>
+        <v>300</v>
+      </c>
+      <c r="I76" s="8">
+        <f t="shared" si="9"/>
+        <v>60.627379999999995</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C77" s="6">
+        <v>19</v>
+      </c>
+      <c r="D77" s="7">
+        <v>4</v>
+      </c>
+      <c r="E77" s="7">
+        <v>0.66993829999999999</v>
+      </c>
+      <c r="G77" s="8">
+        <f t="shared" si="7"/>
+        <v>1900</v>
+      </c>
+      <c r="H77" s="8">
+        <f t="shared" si="8"/>
+        <v>400</v>
+      </c>
+      <c r="I77" s="8">
+        <f t="shared" si="9"/>
+        <v>66.993830000000003</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C78" s="6">
+        <v>25</v>
+      </c>
+      <c r="D78" s="7">
+        <v>5</v>
+      </c>
+      <c r="E78" s="7">
+        <v>0.46792899999999998</v>
+      </c>
+      <c r="G78" s="8">
+        <f t="shared" si="7"/>
+        <v>2500</v>
+      </c>
+      <c r="H78" s="8">
+        <f t="shared" si="8"/>
+        <v>500</v>
+      </c>
+      <c r="I78" s="8">
+        <f t="shared" si="9"/>
+        <v>46.792899999999996</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C79" s="6">
+        <v>20</v>
+      </c>
+      <c r="D79" s="7">
+        <v>6</v>
+      </c>
+      <c r="E79" s="7">
+        <v>0.59172519999999995</v>
+      </c>
+      <c r="G79" s="8">
+        <f t="shared" si="7"/>
+        <v>2000</v>
+      </c>
+      <c r="H79" s="8">
+        <f t="shared" si="8"/>
+        <v>600</v>
+      </c>
+      <c r="I79" s="8">
+        <f t="shared" si="9"/>
+        <v>59.172519999999992</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C80" s="6">
+        <v>2</v>
+      </c>
+      <c r="D80" s="7">
+        <v>7</v>
+      </c>
+      <c r="E80" s="7">
+        <v>0.59955990000000003</v>
+      </c>
+      <c r="G80" s="8">
+        <f t="shared" si="7"/>
+        <v>200</v>
+      </c>
+      <c r="H80" s="8">
+        <f t="shared" si="8"/>
+        <v>700</v>
+      </c>
+      <c r="I80" s="8">
+        <f t="shared" si="9"/>
+        <v>59.95599</v>
+      </c>
+    </row>
+    <row r="81" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C81" s="6">
+        <v>21</v>
+      </c>
+      <c r="D81" s="7">
+        <v>8</v>
+      </c>
+      <c r="E81" s="7">
+        <v>0.59209509999999999</v>
+      </c>
+      <c r="G81" s="8">
+        <f t="shared" si="7"/>
+        <v>2100</v>
+      </c>
+      <c r="H81" s="8">
+        <f t="shared" si="8"/>
+        <v>800</v>
+      </c>
+      <c r="I81" s="8">
+        <f t="shared" si="9"/>
+        <v>59.209510000000002</v>
+      </c>
+    </row>
+    <row r="82" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C82" s="6">
+        <v>22</v>
+      </c>
+      <c r="D82" s="7">
+        <v>9</v>
+      </c>
+      <c r="E82" s="7">
+        <v>0.60197129999999999</v>
+      </c>
+      <c r="G82" s="8">
+        <f t="shared" si="7"/>
+        <v>2200</v>
+      </c>
+      <c r="H82" s="8">
+        <f t="shared" si="8"/>
+        <v>900</v>
+      </c>
+      <c r="I82" s="8">
+        <f t="shared" si="9"/>
+        <v>60.197130000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C83" s="6">
+        <v>3</v>
+      </c>
+      <c r="D83" s="7">
+        <v>10</v>
+      </c>
+      <c r="E83" s="7">
+        <v>0.6120911</v>
+      </c>
+      <c r="G83" s="8">
+        <f t="shared" si="7"/>
+        <v>300</v>
+      </c>
+      <c r="H83" s="8">
+        <f t="shared" si="8"/>
+        <v>1000</v>
+      </c>
+      <c r="I83" s="8">
+        <f t="shared" si="9"/>
+        <v>61.209110000000003</v>
+      </c>
+    </row>
+    <row r="84" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C84" s="6">
+        <v>31</v>
+      </c>
+      <c r="D84" s="7">
+        <v>11</v>
+      </c>
+      <c r="E84" s="7">
+        <v>0.2686885</v>
+      </c>
+      <c r="G84" s="8">
+        <f t="shared" si="7"/>
+        <v>3100</v>
+      </c>
+      <c r="H84" s="8">
+        <f t="shared" si="8"/>
+        <v>1100</v>
+      </c>
+      <c r="I84" s="8">
+        <f t="shared" si="9"/>
+        <v>26.868849999999998</v>
+      </c>
+    </row>
+    <row r="85" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C85" s="6">
+        <v>26</v>
+      </c>
+      <c r="D85" s="7">
+        <v>12</v>
+      </c>
+      <c r="E85" s="7">
+        <v>0.50850709999999999</v>
+      </c>
+      <c r="G85" s="8">
+        <f t="shared" si="7"/>
+        <v>2600</v>
+      </c>
+      <c r="H85" s="8">
+        <f t="shared" si="8"/>
+        <v>1200</v>
+      </c>
+      <c r="I85" s="8">
+        <f t="shared" si="9"/>
+        <v>50.850709999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C86" s="6">
+        <v>14</v>
+      </c>
+      <c r="D86" s="7">
+        <v>13</v>
+      </c>
+      <c r="E86" s="7">
+        <v>0.51265150000000004</v>
+      </c>
+      <c r="G86" s="8">
+        <f t="shared" si="7"/>
+        <v>1400</v>
+      </c>
+      <c r="H86" s="8">
+        <f t="shared" si="8"/>
+        <v>1300</v>
+      </c>
+      <c r="I86" s="8">
+        <f t="shared" si="9"/>
+        <v>51.265150000000006</v>
+      </c>
+    </row>
+    <row r="87" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C87" s="6">
+        <v>15</v>
+      </c>
+      <c r="D87" s="7">
+        <v>14</v>
+      </c>
+      <c r="E87" s="7">
+        <v>0.45423019999999997</v>
+      </c>
+      <c r="G87" s="8">
+        <f t="shared" si="7"/>
+        <v>1500</v>
+      </c>
+      <c r="H87" s="8">
+        <f t="shared" si="8"/>
+        <v>1400</v>
+      </c>
+      <c r="I87" s="8">
+        <f t="shared" si="9"/>
+        <v>45.423019999999994</v>
+      </c>
+    </row>
+    <row r="88" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C88" s="6">
+        <v>27</v>
+      </c>
+      <c r="D88" s="7">
+        <v>15</v>
+      </c>
+      <c r="E88" s="7">
+        <v>0.55507600000000001</v>
+      </c>
+      <c r="G88" s="8">
+        <f t="shared" si="7"/>
+        <v>2700</v>
+      </c>
+      <c r="H88" s="8">
+        <f t="shared" si="8"/>
+        <v>1500</v>
+      </c>
+      <c r="I88" s="8">
+        <f t="shared" si="9"/>
+        <v>55.507600000000004</v>
+      </c>
+    </row>
+    <row r="89" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C89" s="6">
+        <v>23</v>
+      </c>
+      <c r="D89" s="7">
+        <v>16</v>
+      </c>
+      <c r="E89" s="7">
+        <v>0.52100970000000002</v>
+      </c>
+      <c r="G89" s="8">
+        <f t="shared" si="7"/>
+        <v>2300</v>
+      </c>
+      <c r="H89" s="8">
+        <f t="shared" si="8"/>
+        <v>1600</v>
+      </c>
+      <c r="I89" s="8">
+        <f t="shared" si="9"/>
+        <v>52.100970000000004</v>
+      </c>
+    </row>
+    <row r="90" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C90" s="6">
+        <v>9</v>
+      </c>
+      <c r="D90" s="7">
+        <v>17</v>
+      </c>
+      <c r="E90" s="7">
+        <v>0.66382830000000004</v>
+      </c>
+      <c r="G90" s="8">
+        <f t="shared" si="7"/>
+        <v>900</v>
+      </c>
+      <c r="H90" s="8">
+        <f t="shared" si="8"/>
+        <v>1700</v>
+      </c>
+      <c r="I90" s="8">
+        <f t="shared" si="9"/>
+        <v>66.382829999999998</v>
+      </c>
+    </row>
+    <row r="91" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C91" s="6">
+        <v>16</v>
+      </c>
+      <c r="D91" s="7">
+        <v>18</v>
+      </c>
+      <c r="E91" s="7">
+        <v>0.51313719999999996</v>
+      </c>
+      <c r="G91" s="8">
+        <f t="shared" si="7"/>
+        <v>1600</v>
+      </c>
+      <c r="H91" s="8">
+        <f t="shared" si="8"/>
+        <v>1800</v>
+      </c>
+      <c r="I91" s="8">
+        <f t="shared" si="9"/>
+        <v>51.313719999999996</v>
+      </c>
+    </row>
+    <row r="92" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C92" s="6">
+        <v>17</v>
+      </c>
+      <c r="D92" s="7">
+        <v>19</v>
+      </c>
+      <c r="E92" s="7">
+        <v>0.42961300000000002</v>
+      </c>
+      <c r="G92" s="8">
+        <f t="shared" si="7"/>
+        <v>1700</v>
+      </c>
+      <c r="H92" s="8">
+        <f t="shared" si="8"/>
+        <v>1900</v>
+      </c>
+      <c r="I92" s="8">
+        <f t="shared" si="9"/>
+        <v>42.961300000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C93" s="6">
+        <v>18</v>
+      </c>
+      <c r="D93" s="7">
+        <v>20</v>
+      </c>
+      <c r="E93" s="7">
+        <v>0.52924190000000004</v>
+      </c>
+      <c r="G93" s="8">
+        <f t="shared" si="7"/>
+        <v>1800</v>
+      </c>
+      <c r="H93" s="8">
+        <f t="shared" si="8"/>
+        <v>2000</v>
+      </c>
+      <c r="I93" s="8">
+        <f t="shared" si="9"/>
+        <v>52.924190000000003</v>
+      </c>
+    </row>
+    <row r="94" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C94" s="6">
+        <v>13</v>
+      </c>
+      <c r="D94" s="7">
+        <v>21</v>
+      </c>
+      <c r="E94" s="7">
+        <v>0.62787689999999996</v>
+      </c>
+      <c r="G94" s="8">
+        <f t="shared" si="7"/>
+        <v>1300</v>
+      </c>
+      <c r="H94" s="8">
+        <f t="shared" si="8"/>
+        <v>2100</v>
+      </c>
+      <c r="I94" s="8">
+        <f t="shared" si="9"/>
+        <v>62.787689999999998</v>
+      </c>
+    </row>
+    <row r="95" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C95" s="6">
+        <v>4</v>
+      </c>
+      <c r="D95" s="7">
+        <v>22</v>
+      </c>
+      <c r="E95" s="7">
+        <v>0.60075350000000005</v>
+      </c>
+      <c r="G95" s="8">
+        <f t="shared" si="7"/>
+        <v>400</v>
+      </c>
+      <c r="H95" s="8">
+        <f t="shared" si="8"/>
+        <v>2200</v>
+      </c>
+      <c r="I95" s="8">
+        <f t="shared" si="9"/>
+        <v>60.075350000000007</v>
+      </c>
+    </row>
+    <row r="96" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C96" s="6">
+        <v>1</v>
+      </c>
+      <c r="D96" s="7">
+        <v>23</v>
+      </c>
+      <c r="E96" s="7">
+        <v>0.77473749999999997</v>
+      </c>
+      <c r="G96" s="8">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="H96" s="8">
+        <f t="shared" si="8"/>
+        <v>2300</v>
+      </c>
+      <c r="I96" s="8">
+        <f t="shared" si="9"/>
+        <v>77.473749999999995</v>
+      </c>
+    </row>
+    <row r="97" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C97" s="6">
+        <v>24</v>
+      </c>
+      <c r="D97" s="7">
+        <v>24</v>
+      </c>
+      <c r="E97" s="7">
+        <v>0.60607619999999995</v>
+      </c>
+      <c r="G97" s="8">
+        <f t="shared" si="7"/>
+        <v>2400</v>
+      </c>
+      <c r="H97" s="8">
+        <f t="shared" si="8"/>
+        <v>2400</v>
+      </c>
+      <c r="I97" s="8">
+        <f t="shared" si="9"/>
+        <v>60.607619999999997</v>
+      </c>
+    </row>
+    <row r="98" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C98" s="6">
+        <v>10</v>
+      </c>
+      <c r="D98" s="7">
+        <v>25</v>
+      </c>
+      <c r="E98" s="7">
+        <v>0.66317899999999996</v>
+      </c>
+      <c r="G98" s="8">
+        <f t="shared" si="7"/>
+        <v>1000</v>
+      </c>
+      <c r="H98" s="8">
+        <f t="shared" si="8"/>
+        <v>2500</v>
+      </c>
+      <c r="I98" s="8">
+        <f t="shared" si="9"/>
+        <v>66.317899999999995</v>
+      </c>
+    </row>
+    <row r="99" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C99" s="6">
+        <v>11</v>
+      </c>
+      <c r="D99" s="7">
+        <v>26</v>
+      </c>
+      <c r="E99" s="7">
+        <v>0.71709529999999999</v>
+      </c>
+      <c r="G99" s="8">
+        <f t="shared" si="7"/>
+        <v>1100</v>
+      </c>
+      <c r="H99" s="8">
+        <f t="shared" si="8"/>
+        <v>2600</v>
+      </c>
+      <c r="I99" s="8">
+        <f t="shared" si="9"/>
+        <v>71.709530000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C100" s="6">
+        <v>28</v>
+      </c>
+      <c r="D100" s="7">
+        <v>27</v>
+      </c>
+      <c r="E100" s="7">
+        <v>0.56019249999999998</v>
+      </c>
+      <c r="G100" s="8">
+        <f t="shared" si="7"/>
+        <v>2800</v>
+      </c>
+      <c r="H100" s="8">
+        <f t="shared" si="8"/>
+        <v>2700</v>
+      </c>
+      <c r="I100" s="8">
+        <f t="shared" si="9"/>
+        <v>56.01925</v>
+      </c>
+    </row>
+    <row r="101" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C101" s="6">
+        <v>29</v>
+      </c>
+      <c r="D101" s="7">
+        <v>28</v>
+      </c>
+      <c r="E101" s="7">
+        <v>0.63732489999999997</v>
+      </c>
+      <c r="G101" s="8">
+        <f t="shared" si="7"/>
+        <v>2900</v>
+      </c>
+      <c r="H101" s="8">
+        <f t="shared" si="8"/>
+        <v>2800</v>
+      </c>
+      <c r="I101" s="8">
+        <f t="shared" si="9"/>
+        <v>63.732489999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C102" s="6">
+        <v>30</v>
+      </c>
+      <c r="D102" s="7">
+        <v>29</v>
+      </c>
+      <c r="E102" s="7">
+        <v>0.55723679999999998</v>
+      </c>
+      <c r="G102" s="8">
+        <f t="shared" si="7"/>
+        <v>3000</v>
+      </c>
+      <c r="H102" s="8">
+        <f t="shared" si="8"/>
+        <v>2900</v>
+      </c>
+      <c r="I102" s="8">
+        <f t="shared" si="9"/>
+        <v>55.723679999999995</v>
+      </c>
+    </row>
+    <row r="103" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C103" s="6">
+        <v>5</v>
+      </c>
+      <c r="D103" s="7">
+        <v>30</v>
+      </c>
+      <c r="E103" s="7">
+        <v>0.87563389999999997</v>
+      </c>
+      <c r="G103" s="8">
+        <f t="shared" si="7"/>
+        <v>500</v>
+      </c>
+      <c r="H103" s="8">
+        <f t="shared" si="8"/>
+        <v>3000</v>
+      </c>
+      <c r="I103" s="8">
+        <f t="shared" si="9"/>
+        <v>87.563389999999998</v>
+      </c>
+    </row>
+    <row r="104" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G104" s="8">
+        <f t="shared" ref="G104:G137" si="10">C104*100</f>
+        <v>0</v>
+      </c>
+      <c r="H104" s="8">
+        <f t="shared" ref="H104:H137" si="11">D104*100</f>
+        <v>0</v>
+      </c>
+      <c r="I104" s="8">
+        <f t="shared" ref="I104:I137" si="12">E104*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="3:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C105" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G105" s="8" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H105" s="8" t="e">
+        <f t="shared" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I105" s="8">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+      <c r="G106" s="8">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H106" s="8">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="I106" s="8">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="3:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C107" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G107" s="8" t="e">
+        <f t="shared" ref="G107:G139" si="13">C107*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H107" s="8" t="e">
+        <f t="shared" ref="H107:H139" si="14">D107*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I107" s="8">
+        <f t="shared" ref="I107:I139" si="15">E107*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
+      <c r="G108" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H108" s="8">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="I108" s="8">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C109" s="6">
+        <v>6</v>
+      </c>
+      <c r="D109" s="7">
+        <v>0</v>
+      </c>
+      <c r="E109" s="7">
+        <v>0.33411091999999998</v>
+      </c>
+      <c r="G109" s="8">
+        <f t="shared" si="13"/>
+        <v>600</v>
+      </c>
+      <c r="H109" s="8">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="I109" s="8">
+        <f t="shared" si="15"/>
+        <v>33.411091999999996</v>
+      </c>
+    </row>
+    <row r="110" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C110" s="6">
+        <v>7</v>
+      </c>
+      <c r="D110" s="7">
+        <v>1</v>
+      </c>
+      <c r="E110" s="7">
+        <v>0.41044543</v>
+      </c>
+      <c r="G110" s="8">
+        <f t="shared" si="13"/>
+        <v>700</v>
+      </c>
+      <c r="H110" s="8">
+        <f t="shared" si="14"/>
+        <v>100</v>
+      </c>
+      <c r="I110" s="8">
+        <f t="shared" si="15"/>
+        <v>41.044542999999997</v>
+      </c>
+    </row>
+    <row r="111" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C111" s="6">
+        <v>8</v>
+      </c>
+      <c r="D111" s="7">
+        <v>2</v>
+      </c>
+      <c r="E111" s="7">
+        <v>0.25628543999999998</v>
+      </c>
+      <c r="G111" s="8">
+        <f t="shared" si="13"/>
+        <v>800</v>
+      </c>
+      <c r="H111" s="8">
+        <f t="shared" si="14"/>
+        <v>200</v>
+      </c>
+      <c r="I111" s="8">
+        <f t="shared" si="15"/>
+        <v>25.628543999999998</v>
+      </c>
+    </row>
+    <row r="112" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C112" s="6">
+        <v>12</v>
+      </c>
+      <c r="D112" s="7">
+        <v>3</v>
+      </c>
+      <c r="E112" s="7">
+        <v>0.27915366000000003</v>
+      </c>
+      <c r="G112" s="8">
+        <f t="shared" si="13"/>
+        <v>1200</v>
+      </c>
+      <c r="H112" s="8">
+        <f t="shared" si="14"/>
+        <v>300</v>
+      </c>
+      <c r="I112" s="8">
+        <f t="shared" si="15"/>
+        <v>27.915366000000002</v>
+      </c>
+    </row>
+    <row r="113" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C113" s="6">
+        <v>19</v>
+      </c>
+      <c r="D113" s="7">
+        <v>4</v>
+      </c>
+      <c r="E113" s="7">
+        <v>0.13956668</v>
+      </c>
+      <c r="G113" s="8">
+        <f t="shared" si="13"/>
+        <v>1900</v>
+      </c>
+      <c r="H113" s="8">
+        <f t="shared" si="14"/>
+        <v>400</v>
+      </c>
+      <c r="I113" s="8">
+        <f t="shared" si="15"/>
+        <v>13.956668000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C114" s="6">
+        <v>25</v>
+      </c>
+      <c r="D114" s="7">
+        <v>5</v>
+      </c>
+      <c r="E114" s="7">
+        <v>0.51426035999999997</v>
+      </c>
+      <c r="G114" s="8">
+        <f t="shared" si="13"/>
+        <v>2500</v>
+      </c>
+      <c r="H114" s="8">
+        <f t="shared" si="14"/>
+        <v>500</v>
+      </c>
+      <c r="I114" s="8">
+        <f t="shared" si="15"/>
+        <v>51.426035999999996</v>
+      </c>
+    </row>
+    <row r="115" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C115" s="6">
+        <v>20</v>
+      </c>
+      <c r="D115" s="7">
+        <v>6</v>
+      </c>
+      <c r="E115" s="7">
+        <v>0.33899267</v>
+      </c>
+      <c r="G115" s="8">
+        <f t="shared" si="13"/>
+        <v>2000</v>
+      </c>
+      <c r="H115" s="8">
+        <f t="shared" si="14"/>
+        <v>600</v>
+      </c>
+      <c r="I115" s="8">
+        <f t="shared" si="15"/>
+        <v>33.899267000000002</v>
+      </c>
+    </row>
+    <row r="116" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C116" s="6">
+        <v>2</v>
+      </c>
+      <c r="D116" s="7">
+        <v>7</v>
+      </c>
+      <c r="E116" s="7">
+        <v>0.32208131000000001</v>
+      </c>
+      <c r="G116" s="8">
+        <f t="shared" si="13"/>
+        <v>200</v>
+      </c>
+      <c r="H116" s="8">
+        <f t="shared" si="14"/>
+        <v>700</v>
+      </c>
+      <c r="I116" s="8">
+        <f t="shared" si="15"/>
+        <v>32.208131000000002</v>
+      </c>
+    </row>
+    <row r="117" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C117" s="6">
+        <v>21</v>
+      </c>
+      <c r="D117" s="7">
+        <v>8</v>
+      </c>
+      <c r="E117" s="7">
+        <v>0.38577001999999999</v>
+      </c>
+      <c r="G117" s="8">
+        <f t="shared" si="13"/>
+        <v>2100</v>
+      </c>
+      <c r="H117" s="8">
+        <f t="shared" si="14"/>
+        <v>800</v>
+      </c>
+      <c r="I117" s="8">
+        <f t="shared" si="15"/>
+        <v>38.577002</v>
+      </c>
+    </row>
+    <row r="118" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C118" s="6">
+        <v>22</v>
+      </c>
+      <c r="D118" s="7">
+        <v>9</v>
+      </c>
+      <c r="E118" s="7">
+        <v>0.26299974999999998</v>
+      </c>
+      <c r="G118" s="8">
+        <f t="shared" si="13"/>
+        <v>2200</v>
+      </c>
+      <c r="H118" s="8">
+        <f t="shared" si="14"/>
+        <v>900</v>
+      </c>
+      <c r="I118" s="8">
+        <f t="shared" si="15"/>
+        <v>26.299974999999996</v>
+      </c>
+    </row>
+    <row r="119" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C119" s="6">
+        <v>3</v>
+      </c>
+      <c r="D119" s="7">
+        <v>10</v>
+      </c>
+      <c r="E119" s="7">
+        <v>0.35960723999999999</v>
+      </c>
+      <c r="G119" s="8">
+        <f t="shared" si="13"/>
+        <v>300</v>
+      </c>
+      <c r="H119" s="8">
+        <f t="shared" si="14"/>
+        <v>1000</v>
+      </c>
+      <c r="I119" s="8">
+        <f t="shared" si="15"/>
+        <v>35.960723999999999</v>
+      </c>
+    </row>
+    <row r="120" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C120" s="6">
+        <v>31</v>
+      </c>
+      <c r="D120" s="7">
+        <v>11</v>
+      </c>
+      <c r="E120" s="7">
+        <v>0.27714832</v>
+      </c>
+      <c r="G120" s="8">
+        <f t="shared" si="13"/>
+        <v>3100</v>
+      </c>
+      <c r="H120" s="8">
+        <f t="shared" si="14"/>
+        <v>1100</v>
+      </c>
+      <c r="I120" s="8">
+        <f t="shared" si="15"/>
+        <v>27.714832000000001</v>
+      </c>
+    </row>
+    <row r="121" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C121" s="6">
+        <v>26</v>
+      </c>
+      <c r="D121" s="7">
+        <v>12</v>
+      </c>
+      <c r="E121" s="7">
+        <v>0.39178417999999998</v>
+      </c>
+      <c r="G121" s="8">
+        <f t="shared" si="13"/>
+        <v>2600</v>
+      </c>
+      <c r="H121" s="8">
+        <f t="shared" si="14"/>
+        <v>1200</v>
+      </c>
+      <c r="I121" s="8">
+        <f t="shared" si="15"/>
+        <v>39.178418000000001</v>
+      </c>
+    </row>
+    <row r="122" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C122" s="6">
+        <v>14</v>
+      </c>
+      <c r="D122" s="7">
+        <v>13</v>
+      </c>
+      <c r="E122" s="7">
+        <v>0.37383604999999998</v>
+      </c>
+      <c r="G122" s="8">
+        <f t="shared" si="13"/>
+        <v>1400</v>
+      </c>
+      <c r="H122" s="8">
+        <f t="shared" si="14"/>
+        <v>1300</v>
+      </c>
+      <c r="I122" s="8">
+        <f t="shared" si="15"/>
+        <v>37.383604999999996</v>
+      </c>
+    </row>
+    <row r="123" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C123" s="6">
+        <v>15</v>
+      </c>
+      <c r="D123" s="7">
+        <v>14</v>
+      </c>
+      <c r="E123" s="7">
+        <v>0.29334258000000002</v>
+      </c>
+      <c r="G123" s="8">
+        <f t="shared" si="13"/>
+        <v>1500</v>
+      </c>
+      <c r="H123" s="8">
+        <f t="shared" si="14"/>
+        <v>1400</v>
+      </c>
+      <c r="I123" s="8">
+        <f t="shared" si="15"/>
+        <v>29.334258000000002</v>
+      </c>
+    </row>
+    <row r="124" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C124" s="6">
+        <v>27</v>
+      </c>
+      <c r="D124" s="7">
+        <v>15</v>
+      </c>
+      <c r="E124" s="7">
+        <v>0.39750829999999998</v>
+      </c>
+      <c r="G124" s="8">
+        <f t="shared" si="13"/>
+        <v>2700</v>
+      </c>
+      <c r="H124" s="8">
+        <f t="shared" si="14"/>
+        <v>1500</v>
+      </c>
+      <c r="I124" s="8">
+        <f t="shared" si="15"/>
+        <v>39.750830000000001</v>
+      </c>
+    </row>
+    <row r="125" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C125" s="6">
+        <v>23</v>
+      </c>
+      <c r="D125" s="7">
+        <v>16</v>
+      </c>
+      <c r="E125" s="7">
+        <v>0.4731997</v>
+      </c>
+      <c r="G125" s="8">
+        <f t="shared" si="13"/>
+        <v>2300</v>
+      </c>
+      <c r="H125" s="8">
+        <f t="shared" si="14"/>
+        <v>1600</v>
+      </c>
+      <c r="I125" s="8">
+        <f t="shared" si="15"/>
+        <v>47.319969999999998</v>
+      </c>
+    </row>
+    <row r="126" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C126" s="6">
+        <v>9</v>
+      </c>
+      <c r="D126" s="7">
+        <v>17</v>
+      </c>
+      <c r="E126" s="7">
+        <v>0.33617164999999999</v>
+      </c>
+      <c r="G126" s="8">
+        <f t="shared" si="13"/>
+        <v>900</v>
+      </c>
+      <c r="H126" s="8">
+        <f t="shared" si="14"/>
+        <v>1700</v>
+      </c>
+      <c r="I126" s="8">
+        <f t="shared" si="15"/>
+        <v>33.617165</v>
+      </c>
+    </row>
+    <row r="127" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C127" s="6">
+        <v>16</v>
+      </c>
+      <c r="D127" s="7">
+        <v>18</v>
+      </c>
+      <c r="E127" s="7">
+        <v>0.39590834000000003</v>
+      </c>
+      <c r="G127" s="8">
+        <f t="shared" si="13"/>
+        <v>1600</v>
+      </c>
+      <c r="H127" s="8">
+        <f t="shared" si="14"/>
+        <v>1800</v>
+      </c>
+      <c r="I127" s="8">
+        <f t="shared" si="15"/>
+        <v>39.590834000000001</v>
+      </c>
+    </row>
+    <row r="128" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C128" s="6">
+        <v>17</v>
+      </c>
+      <c r="D128" s="7">
+        <v>19</v>
+      </c>
+      <c r="E128" s="7">
+        <v>0.51664849999999996</v>
+      </c>
+      <c r="G128" s="8">
+        <f t="shared" si="13"/>
+        <v>1700</v>
+      </c>
+      <c r="H128" s="8">
+        <f t="shared" si="14"/>
+        <v>1900</v>
+      </c>
+      <c r="I128" s="8">
+        <f t="shared" si="15"/>
+        <v>51.664849999999994</v>
+      </c>
+    </row>
+    <row r="129" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C129" s="6">
+        <v>18</v>
+      </c>
+      <c r="D129" s="7">
+        <v>20</v>
+      </c>
+      <c r="E129" s="7">
+        <v>0.46667621999999997</v>
+      </c>
+      <c r="G129" s="8">
+        <f t="shared" si="13"/>
+        <v>1800</v>
+      </c>
+      <c r="H129" s="8">
+        <f t="shared" si="14"/>
+        <v>2000</v>
+      </c>
+      <c r="I129" s="8">
+        <f t="shared" si="15"/>
+        <v>46.667621999999994</v>
+      </c>
+    </row>
+    <row r="130" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C130" s="6">
+        <v>13</v>
+      </c>
+      <c r="D130" s="7">
+        <v>21</v>
+      </c>
+      <c r="E130" s="7">
+        <v>0.31059821999999998</v>
+      </c>
+      <c r="G130" s="8">
+        <f t="shared" si="13"/>
+        <v>1300</v>
+      </c>
+      <c r="H130" s="8">
+        <f t="shared" si="14"/>
+        <v>2100</v>
+      </c>
+      <c r="I130" s="8">
+        <f t="shared" si="15"/>
+        <v>31.059821999999997</v>
+      </c>
+    </row>
+    <row r="131" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C131" s="6">
+        <v>4</v>
+      </c>
+      <c r="D131" s="7">
+        <v>22</v>
+      </c>
+      <c r="E131" s="7">
+        <v>0.27583531</v>
+      </c>
+      <c r="G131" s="8">
+        <f t="shared" si="13"/>
+        <v>400</v>
+      </c>
+      <c r="H131" s="8">
+        <f t="shared" si="14"/>
+        <v>2200</v>
+      </c>
+      <c r="I131" s="8">
+        <f t="shared" si="15"/>
+        <v>27.583531000000001</v>
+      </c>
+    </row>
+    <row r="132" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C132" s="6">
+        <v>1</v>
+      </c>
+      <c r="D132" s="7">
+        <v>23</v>
+      </c>
+      <c r="E132" s="7">
+        <v>0.12453996000000001</v>
+      </c>
+      <c r="G132" s="8">
+        <f t="shared" si="13"/>
+        <v>100</v>
+      </c>
+      <c r="H132" s="8">
+        <f t="shared" si="14"/>
+        <v>2300</v>
+      </c>
+      <c r="I132" s="8">
+        <f t="shared" si="15"/>
+        <v>12.453996</v>
+      </c>
+    </row>
+    <row r="133" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C133" s="6">
+        <v>24</v>
+      </c>
+      <c r="D133" s="7">
+        <v>24</v>
+      </c>
+      <c r="E133" s="7">
+        <v>0.25853448000000001</v>
+      </c>
+      <c r="G133" s="8">
+        <f t="shared" si="13"/>
+        <v>2400</v>
+      </c>
+      <c r="H133" s="8">
+        <f t="shared" si="14"/>
+        <v>2400</v>
+      </c>
+      <c r="I133" s="8">
+        <f t="shared" si="15"/>
+        <v>25.853448</v>
+      </c>
+    </row>
+    <row r="134" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C134" s="6">
+        <v>10</v>
+      </c>
+      <c r="D134" s="7">
+        <v>25</v>
+      </c>
+      <c r="E134" s="7">
+        <v>0.26233972999999999</v>
+      </c>
+      <c r="G134" s="8">
+        <f t="shared" si="13"/>
+        <v>1000</v>
+      </c>
+      <c r="H134" s="8">
+        <f t="shared" si="14"/>
+        <v>2500</v>
+      </c>
+      <c r="I134" s="8">
+        <f t="shared" si="15"/>
+        <v>26.233972999999999</v>
+      </c>
+    </row>
+    <row r="135" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C135" s="6">
+        <v>11</v>
+      </c>
+      <c r="D135" s="7">
+        <v>26</v>
+      </c>
+      <c r="E135" s="7">
+        <v>0.19270863999999999</v>
+      </c>
+      <c r="G135" s="8">
+        <f t="shared" si="13"/>
+        <v>1100</v>
+      </c>
+      <c r="H135" s="8">
+        <f t="shared" si="14"/>
+        <v>2600</v>
+      </c>
+      <c r="I135" s="8">
+        <f t="shared" si="15"/>
+        <v>19.270864</v>
+      </c>
+    </row>
+    <row r="136" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C136" s="6">
+        <v>28</v>
+      </c>
+      <c r="D136" s="7">
+        <v>27</v>
+      </c>
+      <c r="E136" s="7">
+        <v>0.38802697000000003</v>
+      </c>
+      <c r="G136" s="8">
+        <f t="shared" si="13"/>
+        <v>2800</v>
+      </c>
+      <c r="H136" s="8">
+        <f t="shared" si="14"/>
+        <v>2700</v>
+      </c>
+      <c r="I136" s="8">
+        <f t="shared" si="15"/>
+        <v>38.802697000000002</v>
+      </c>
+    </row>
+    <row r="137" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C137" s="6">
+        <v>29</v>
+      </c>
+      <c r="D137" s="7">
+        <v>28</v>
+      </c>
+      <c r="E137" s="7">
+        <v>0.32456657999999999</v>
+      </c>
+      <c r="G137" s="8">
+        <f t="shared" si="13"/>
+        <v>2900</v>
+      </c>
+      <c r="H137" s="8">
+        <f t="shared" si="14"/>
+        <v>2800</v>
+      </c>
+      <c r="I137" s="8">
+        <f t="shared" si="15"/>
+        <v>32.456657999999997</v>
+      </c>
+    </row>
+    <row r="138" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C138" s="6">
+        <v>30</v>
+      </c>
+      <c r="D138" s="7">
+        <v>29</v>
+      </c>
+      <c r="E138" s="7">
+        <v>0.44276315999999999</v>
+      </c>
+      <c r="G138" s="8">
+        <f t="shared" si="13"/>
+        <v>3000</v>
+      </c>
+      <c r="H138" s="8">
+        <f t="shared" si="14"/>
+        <v>2900</v>
+      </c>
+      <c r="I138" s="8">
+        <f t="shared" si="15"/>
+        <v>44.276316000000001</v>
+      </c>
+    </row>
+    <row r="139" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C139" s="6">
+        <v>5</v>
+      </c>
+      <c r="D139" s="7">
+        <v>30</v>
+      </c>
+      <c r="E139" s="7">
+        <v>6.6327979999999995E-2</v>
+      </c>
+      <c r="G139" s="8">
+        <f t="shared" si="13"/>
+        <v>500</v>
+      </c>
+      <c r="H139" s="8">
+        <f t="shared" si="14"/>
+        <v>3000</v>
+      </c>
+      <c r="I139" s="8">
+        <f t="shared" si="15"/>
+        <v>6.6327979999999993</v>
+      </c>
+    </row>
+    <row r="140" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G140" s="8">
+        <f t="shared" ref="G140:G174" si="16">C140*100</f>
+        <v>0</v>
+      </c>
+      <c r="H140" s="8">
+        <f t="shared" ref="H140:H174" si="17">D140*100</f>
+        <v>0</v>
+      </c>
+      <c r="I140" s="8">
+        <f t="shared" ref="I140:I174" si="18">E140*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G141" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="H141" s="8">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="I141" s="8">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="3:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C142" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D142" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G142" s="8" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H142" s="8" t="e">
+        <f t="shared" si="17"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I142" s="8">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C143" s="5"/>
+      <c r="D143" s="5"/>
+      <c r="E143" s="5"/>
+      <c r="G143" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="H143" s="8">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="I143" s="8">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C144" s="6">
+        <v>1</v>
+      </c>
+      <c r="D144" s="7">
+        <v>0</v>
+      </c>
+      <c r="E144" s="7">
+        <v>0.10869384999999999</v>
+      </c>
+      <c r="G144" s="8">
+        <f t="shared" si="16"/>
+        <v>100</v>
+      </c>
+      <c r="H144" s="8">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="I144" s="8">
+        <f t="shared" si="18"/>
+        <v>10.869384999999999</v>
+      </c>
+    </row>
+    <row r="145" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C145" s="6">
+        <v>2</v>
+      </c>
+      <c r="D145" s="7">
+        <v>1</v>
+      </c>
+      <c r="E145" s="7">
+        <v>0.19506219</v>
+      </c>
+      <c r="G145" s="8">
+        <f t="shared" si="16"/>
+        <v>200</v>
+      </c>
+      <c r="H145" s="8">
+        <f t="shared" si="17"/>
+        <v>100</v>
+      </c>
+      <c r="I145" s="8">
+        <f t="shared" si="18"/>
+        <v>19.506218999999998</v>
+      </c>
+    </row>
+    <row r="146" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C146" s="6">
+        <v>3</v>
+      </c>
+      <c r="D146" s="7">
+        <v>2</v>
+      </c>
+      <c r="E146" s="7">
+        <v>0.11452873</v>
+      </c>
+      <c r="G146" s="8">
+        <f t="shared" si="16"/>
+        <v>300</v>
+      </c>
+      <c r="H146" s="8">
+        <f t="shared" si="17"/>
+        <v>200</v>
+      </c>
+      <c r="I146" s="8">
+        <f t="shared" si="18"/>
+        <v>11.452873</v>
+      </c>
+    </row>
+    <row r="147" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C147" s="6">
+        <v>4</v>
+      </c>
+      <c r="D147" s="7">
+        <v>3</v>
+      </c>
+      <c r="E147" s="7">
+        <v>0.13299620000000001</v>
+      </c>
+      <c r="G147" s="8">
+        <f t="shared" si="16"/>
+        <v>400</v>
+      </c>
+      <c r="H147" s="8">
+        <f t="shared" si="17"/>
+        <v>300</v>
+      </c>
+      <c r="I147" s="8">
+        <f t="shared" si="18"/>
+        <v>13.299620000000001</v>
+      </c>
+    </row>
+    <row r="148" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C148" s="6">
+        <v>5</v>
+      </c>
+      <c r="D148" s="7">
+        <v>4</v>
+      </c>
+      <c r="E148" s="7">
+        <v>7.4562390000000006E-2</v>
+      </c>
+      <c r="G148" s="8">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="H148" s="8">
+        <f t="shared" si="17"/>
+        <v>400</v>
+      </c>
+      <c r="I148" s="8">
+        <f t="shared" si="18"/>
+        <v>7.4562390000000009</v>
+      </c>
+    </row>
+    <row r="149" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C149" s="6">
+        <v>6</v>
+      </c>
+      <c r="D149" s="7">
+        <v>5</v>
+      </c>
+      <c r="E149" s="7">
+        <v>0.30386276000000001</v>
+      </c>
+      <c r="G149" s="8">
+        <f t="shared" si="16"/>
+        <v>600</v>
+      </c>
+      <c r="H149" s="8">
+        <f t="shared" si="17"/>
+        <v>500</v>
+      </c>
+      <c r="I149" s="8">
+        <f t="shared" si="18"/>
+        <v>30.386276000000002</v>
+      </c>
+    </row>
+    <row r="150" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C150" s="6">
+        <v>7</v>
+      </c>
+      <c r="D150" s="7">
+        <v>6</v>
+      </c>
+      <c r="E150" s="7">
+        <v>0.20195813000000001</v>
+      </c>
+      <c r="G150" s="8">
+        <f t="shared" si="16"/>
+        <v>700</v>
+      </c>
+      <c r="H150" s="8">
+        <f t="shared" si="17"/>
+        <v>600</v>
+      </c>
+      <c r="I150" s="8">
+        <f t="shared" si="18"/>
+        <v>20.195813000000001</v>
+      </c>
+    </row>
+    <row r="151" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C151" s="6">
+        <v>8</v>
+      </c>
+      <c r="D151" s="7">
+        <v>7</v>
+      </c>
+      <c r="E151" s="7">
+        <v>0.1391482</v>
+      </c>
+      <c r="G151" s="8">
+        <f t="shared" si="16"/>
+        <v>800</v>
+      </c>
+      <c r="H151" s="8">
+        <f t="shared" si="17"/>
+        <v>700</v>
+      </c>
+      <c r="I151" s="8">
+        <f t="shared" si="18"/>
+        <v>13.914820000000001</v>
+      </c>
+    </row>
+    <row r="152" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C152" s="6">
+        <v>9</v>
+      </c>
+      <c r="D152" s="7">
+        <v>8</v>
+      </c>
+      <c r="E152" s="7">
+        <v>0.13900794</v>
+      </c>
+      <c r="G152" s="8">
+        <f t="shared" si="16"/>
+        <v>900</v>
+      </c>
+      <c r="H152" s="8">
+        <f t="shared" si="17"/>
+        <v>800</v>
+      </c>
+      <c r="I152" s="8">
+        <f t="shared" si="18"/>
+        <v>13.900793999999999</v>
+      </c>
+    </row>
+    <row r="153" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C153" s="6">
+        <v>10</v>
+      </c>
+      <c r="D153" s="7">
+        <v>9</v>
+      </c>
+      <c r="E153" s="7">
+        <v>0.17853105</v>
+      </c>
+      <c r="G153" s="8">
+        <f t="shared" si="16"/>
+        <v>1000</v>
+      </c>
+      <c r="H153" s="8">
+        <f t="shared" si="17"/>
+        <v>900</v>
+      </c>
+      <c r="I153" s="8">
+        <f t="shared" si="18"/>
+        <v>17.853104999999999</v>
+      </c>
+    </row>
+    <row r="154" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C154" s="6">
+        <v>11</v>
+      </c>
+      <c r="D154" s="7">
+        <v>10</v>
+      </c>
+      <c r="E154" s="7">
+        <v>0.14567438999999999</v>
+      </c>
+      <c r="G154" s="8">
+        <f t="shared" si="16"/>
+        <v>1100</v>
+      </c>
+      <c r="H154" s="8">
+        <f t="shared" si="17"/>
+        <v>1000</v>
+      </c>
+      <c r="I154" s="8">
+        <f t="shared" si="18"/>
+        <v>14.567438999999998</v>
+      </c>
+    </row>
+    <row r="155" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C155" s="6">
+        <v>12</v>
+      </c>
+      <c r="D155" s="7">
+        <v>11</v>
+      </c>
+      <c r="E155" s="7">
+        <v>0.25250745000000002</v>
+      </c>
+      <c r="G155" s="8">
+        <f t="shared" si="16"/>
+        <v>1200</v>
+      </c>
+      <c r="H155" s="8">
+        <f t="shared" si="17"/>
+        <v>1100</v>
+      </c>
+      <c r="I155" s="8">
+        <f t="shared" si="18"/>
+        <v>25.250745000000002</v>
+      </c>
+    </row>
+    <row r="156" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C156" s="6">
+        <v>13</v>
+      </c>
+      <c r="D156" s="7">
+        <v>12</v>
+      </c>
+      <c r="E156" s="7">
+        <v>0.23655608</v>
+      </c>
+      <c r="G156" s="8">
+        <f t="shared" si="16"/>
+        <v>1300</v>
+      </c>
+      <c r="H156" s="8">
+        <f t="shared" si="17"/>
+        <v>1200</v>
+      </c>
+      <c r="I156" s="8">
+        <f t="shared" si="18"/>
+        <v>23.655608000000001</v>
+      </c>
+    </row>
+    <row r="157" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C157" s="6">
+        <v>14</v>
+      </c>
+      <c r="D157" s="7">
+        <v>13</v>
+      </c>
+      <c r="E157" s="7">
+        <v>0.24894253</v>
+      </c>
+      <c r="G157" s="8">
+        <f t="shared" si="16"/>
+        <v>1400</v>
+      </c>
+      <c r="H157" s="8">
+        <f t="shared" si="17"/>
+        <v>1300</v>
+      </c>
+      <c r="I157" s="8">
+        <f t="shared" si="18"/>
+        <v>24.894252999999999</v>
+      </c>
+    </row>
+    <row r="158" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C158" s="6">
+        <v>15</v>
+      </c>
+      <c r="D158" s="7">
+        <v>14</v>
+      </c>
+      <c r="E158" s="7">
+        <v>0.22283045000000001</v>
+      </c>
+      <c r="G158" s="8">
+        <f t="shared" si="16"/>
+        <v>1500</v>
+      </c>
+      <c r="H158" s="8">
+        <f t="shared" si="17"/>
+        <v>1400</v>
+      </c>
+      <c r="I158" s="8">
+        <f t="shared" si="18"/>
+        <v>22.283045000000001</v>
+      </c>
+    </row>
+    <row r="159" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C159" s="6">
+        <v>16</v>
+      </c>
+      <c r="D159" s="7">
+        <v>15</v>
+      </c>
+      <c r="E159" s="7">
+        <v>0.21877845000000001</v>
+      </c>
+      <c r="G159" s="8">
+        <f t="shared" si="16"/>
+        <v>1600</v>
+      </c>
+      <c r="H159" s="8">
+        <f t="shared" si="17"/>
+        <v>1500</v>
+      </c>
+      <c r="I159" s="8">
+        <f t="shared" si="18"/>
+        <v>21.877845000000001</v>
+      </c>
+    </row>
+    <row r="160" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C160" s="6">
+        <v>17</v>
+      </c>
+      <c r="D160" s="7">
+        <v>16</v>
+      </c>
+      <c r="E160" s="7">
+        <v>0.17655604</v>
+      </c>
+      <c r="G160" s="8">
+        <f t="shared" si="16"/>
+        <v>1700</v>
+      </c>
+      <c r="H160" s="8">
+        <f t="shared" si="17"/>
+        <v>1600</v>
+      </c>
+      <c r="I160" s="8">
+        <f t="shared" si="18"/>
+        <v>17.655604</v>
+      </c>
+    </row>
+    <row r="161" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C161" s="6">
+        <v>18</v>
+      </c>
+      <c r="D161" s="7">
+        <v>17</v>
+      </c>
+      <c r="E161" s="7">
+        <v>0.23418201</v>
+      </c>
+      <c r="G161" s="8">
+        <f t="shared" si="16"/>
+        <v>1800</v>
+      </c>
+      <c r="H161" s="8">
+        <f t="shared" si="17"/>
+        <v>1700</v>
+      </c>
+      <c r="I161" s="8">
+        <f t="shared" si="18"/>
+        <v>23.418201</v>
+      </c>
+    </row>
+    <row r="162" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C162" s="6">
+        <v>19</v>
+      </c>
+      <c r="D162" s="7">
+        <v>18</v>
+      </c>
+      <c r="E162" s="7">
+        <v>0.19534926999999999</v>
+      </c>
+      <c r="G162" s="8">
+        <f t="shared" si="16"/>
+        <v>1900</v>
+      </c>
+      <c r="H162" s="8">
+        <f t="shared" si="17"/>
+        <v>1800</v>
+      </c>
+      <c r="I162" s="8">
+        <f t="shared" si="18"/>
+        <v>19.534927</v>
+      </c>
+    </row>
+    <row r="163" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C163" s="6">
+        <v>20</v>
+      </c>
+      <c r="D163" s="7">
+        <v>19</v>
+      </c>
+      <c r="E163" s="7">
+        <v>0.35298889999999999</v>
+      </c>
+      <c r="G163" s="8">
+        <f t="shared" si="16"/>
+        <v>2000</v>
+      </c>
+      <c r="H163" s="8">
+        <f t="shared" si="17"/>
+        <v>1900</v>
+      </c>
+      <c r="I163" s="8">
+        <f t="shared" si="18"/>
+        <v>35.29889</v>
+      </c>
+    </row>
+    <row r="164" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C164" s="6">
+        <v>21</v>
+      </c>
+      <c r="D164" s="7">
+        <v>20</v>
+      </c>
+      <c r="E164" s="7">
+        <v>0.16649578000000001</v>
+      </c>
+      <c r="G164" s="8">
+        <f t="shared" si="16"/>
+        <v>2100</v>
+      </c>
+      <c r="H164" s="8">
+        <f t="shared" si="17"/>
+        <v>2000</v>
+      </c>
+      <c r="I164" s="8">
+        <f t="shared" si="18"/>
+        <v>16.649578000000002</v>
+      </c>
+    </row>
+    <row r="165" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C165" s="6">
+        <v>22</v>
+      </c>
+      <c r="D165" s="7">
+        <v>21</v>
+      </c>
+      <c r="E165" s="7">
+        <v>0.10259122</v>
+      </c>
+      <c r="G165" s="8">
+        <f t="shared" si="16"/>
+        <v>2200</v>
+      </c>
+      <c r="H165" s="8">
+        <f t="shared" si="17"/>
+        <v>2100</v>
+      </c>
+      <c r="I165" s="8">
+        <f t="shared" si="18"/>
+        <v>10.259122</v>
+      </c>
+    </row>
+    <row r="166" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C166" s="6">
+        <v>23</v>
+      </c>
+      <c r="D166" s="7">
+        <v>22</v>
+      </c>
+      <c r="E166" s="7">
+        <v>0.17370774</v>
+      </c>
+      <c r="G166" s="8">
+        <f t="shared" si="16"/>
+        <v>2300</v>
+      </c>
+      <c r="H166" s="8">
+        <f t="shared" si="17"/>
+        <v>2200</v>
+      </c>
+      <c r="I166" s="8">
+        <f t="shared" si="18"/>
+        <v>17.370774000000001</v>
+      </c>
+    </row>
+    <row r="167" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C167" s="6">
+        <v>24</v>
+      </c>
+      <c r="D167" s="7">
+        <v>23</v>
+      </c>
+      <c r="E167" s="7">
+        <v>7.1908879999999994E-2</v>
+      </c>
+      <c r="G167" s="8">
+        <f t="shared" si="16"/>
+        <v>2400</v>
+      </c>
+      <c r="H167" s="8">
+        <f t="shared" si="17"/>
+        <v>2300</v>
+      </c>
+      <c r="I167" s="8">
+        <f t="shared" si="18"/>
+        <v>7.1908879999999993</v>
+      </c>
+    </row>
+    <row r="168" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C168" s="6">
+        <v>25</v>
+      </c>
+      <c r="D168" s="7">
+        <v>24</v>
+      </c>
+      <c r="E168" s="7">
+        <v>0.20268617</v>
+      </c>
+      <c r="G168" s="8">
+        <f t="shared" si="16"/>
+        <v>2500</v>
+      </c>
+      <c r="H168" s="8">
+        <f t="shared" si="17"/>
+        <v>2400</v>
+      </c>
+      <c r="I168" s="8">
+        <f t="shared" si="18"/>
+        <v>20.268616999999999</v>
+      </c>
+    </row>
+    <row r="169" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C169" s="6">
+        <v>26</v>
+      </c>
+      <c r="D169" s="7">
+        <v>25</v>
+      </c>
+      <c r="E169" s="7">
+        <v>0.13336838000000001</v>
+      </c>
+      <c r="G169" s="8">
+        <f t="shared" si="16"/>
+        <v>2600</v>
+      </c>
+      <c r="H169" s="8">
+        <f t="shared" si="17"/>
+        <v>2500</v>
+      </c>
+      <c r="I169" s="8">
+        <f t="shared" si="18"/>
+        <v>13.336838</v>
+      </c>
+    </row>
+    <row r="170" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C170" s="6">
+        <v>27</v>
+      </c>
+      <c r="D170" s="7">
+        <v>26</v>
+      </c>
+      <c r="E170" s="7">
+        <v>0.14249037000000001</v>
+      </c>
+      <c r="G170" s="8">
+        <f t="shared" si="16"/>
+        <v>2700</v>
+      </c>
+      <c r="H170" s="8">
+        <f t="shared" si="17"/>
+        <v>2600</v>
+      </c>
+      <c r="I170" s="8">
+        <f t="shared" si="18"/>
+        <v>14.249037000000001</v>
+      </c>
+    </row>
+    <row r="171" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C171" s="6">
+        <v>28</v>
+      </c>
+      <c r="D171" s="7">
+        <v>27</v>
+      </c>
+      <c r="E171" s="7">
+        <v>0.2131084</v>
+      </c>
+      <c r="G171" s="8">
+        <f t="shared" si="16"/>
+        <v>2800</v>
+      </c>
+      <c r="H171" s="8">
+        <f t="shared" si="17"/>
+        <v>2700</v>
+      </c>
+      <c r="I171" s="8">
+        <f t="shared" si="18"/>
+        <v>21.310839999999999</v>
+      </c>
+    </row>
+    <row r="172" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C172" s="6">
+        <v>29</v>
+      </c>
+      <c r="D172" s="7">
+        <v>28</v>
+      </c>
+      <c r="E172" s="7">
+        <v>0.13478825999999999</v>
+      </c>
+      <c r="G172" s="8">
+        <f t="shared" si="16"/>
+        <v>2900</v>
+      </c>
+      <c r="H172" s="8">
+        <f t="shared" si="17"/>
+        <v>2800</v>
+      </c>
+      <c r="I172" s="8">
+        <f t="shared" si="18"/>
+        <v>13.478826</v>
+      </c>
+    </row>
+    <row r="173" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C173" s="6">
+        <v>30</v>
+      </c>
+      <c r="D173" s="7">
+        <v>29</v>
+      </c>
+      <c r="E173" s="7">
+        <v>0.25987732000000002</v>
+      </c>
+      <c r="G173" s="8">
+        <f t="shared" si="16"/>
+        <v>3000</v>
+      </c>
+      <c r="H173" s="8">
+        <f t="shared" si="17"/>
+        <v>2900</v>
+      </c>
+      <c r="I173" s="8">
+        <f t="shared" si="18"/>
+        <v>25.987732000000001</v>
+      </c>
+    </row>
+    <row r="174" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C174" s="6">
+        <v>31</v>
+      </c>
+      <c r="D174" s="7">
+        <v>30</v>
+      </c>
+      <c r="E174" s="7">
+        <v>7.3343179999999994E-2</v>
+      </c>
+      <c r="G174" s="8">
+        <f t="shared" si="16"/>
+        <v>3100</v>
+      </c>
+      <c r="H174" s="8">
+        <f t="shared" si="17"/>
+        <v>3000</v>
+      </c>
+      <c r="I174" s="8">
+        <f t="shared" si="18"/>
+        <v>7.3343179999999997</v>
+      </c>
+    </row>
+    <row r="175" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G175" s="8">
+        <f t="shared" ref="G175:G209" si="19">C175*100</f>
+        <v>0</v>
+      </c>
+      <c r="H175" s="8">
+        <f t="shared" ref="H175:H209" si="20">D175*100</f>
+        <v>0</v>
+      </c>
+      <c r="I175" s="8">
+        <f t="shared" ref="I175:I209" si="21">E175*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G176" s="8">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H176" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I176" s="8">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="2:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B177" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C177" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F177" s="4"/>
+      <c r="G177" s="8" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H177" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I177" s="8">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B178" s="5"/>
+      <c r="C178" s="5"/>
+      <c r="D178" s="5"/>
+      <c r="E178" s="5"/>
+      <c r="F178" s="5"/>
+      <c r="G178" s="8">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H178" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I178" s="8">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B179" s="6">
+        <v>1</v>
+      </c>
+      <c r="C179" s="7">
+        <v>0</v>
+      </c>
+      <c r="D179" s="7">
+        <v>4.8700719999999996E-3</v>
+      </c>
+      <c r="E179" s="7">
+        <v>0.3252758</v>
+      </c>
+      <c r="F179" s="7"/>
+      <c r="G179" s="8">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H179" s="8">
+        <f t="shared" si="20"/>
+        <v>0.48700719999999997</v>
+      </c>
+      <c r="I179" s="8">
+        <f t="shared" si="21"/>
+        <v>32.52758</v>
+      </c>
+    </row>
+    <row r="180" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B180" s="6">
+        <v>2</v>
+      </c>
+      <c r="C180" s="7">
+        <v>1</v>
+      </c>
+      <c r="D180" s="7">
+        <v>0</v>
+      </c>
+      <c r="E180" s="7">
+        <v>0.1621937</v>
+      </c>
+      <c r="F180" s="7"/>
+      <c r="G180" s="8">
+        <f t="shared" si="19"/>
+        <v>100</v>
+      </c>
+      <c r="H180" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I180" s="8">
+        <f t="shared" si="21"/>
+        <v>16.219369999999998</v>
+      </c>
+    </row>
+    <row r="181" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B181" s="6">
+        <v>3</v>
+      </c>
+      <c r="C181" s="7">
+        <v>2</v>
+      </c>
+      <c r="D181" s="7">
+        <v>0</v>
+      </c>
+      <c r="E181" s="7">
+        <v>0.3132199</v>
+      </c>
+      <c r="F181" s="7"/>
+      <c r="G181" s="8">
+        <f t="shared" si="19"/>
+        <v>200</v>
+      </c>
+      <c r="H181" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I181" s="8">
+        <f t="shared" si="21"/>
+        <v>31.32199</v>
+      </c>
+    </row>
+    <row r="182" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B182" s="6">
+        <v>4</v>
+      </c>
+      <c r="C182" s="7">
+        <v>3</v>
+      </c>
+      <c r="D182" s="7">
+        <v>0</v>
+      </c>
+      <c r="E182" s="7">
+        <v>0.24701200000000001</v>
+      </c>
+      <c r="F182" s="7"/>
+      <c r="G182" s="8">
+        <f t="shared" si="19"/>
+        <v>300</v>
+      </c>
+      <c r="H182" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I182" s="8">
+        <f t="shared" si="21"/>
+        <v>24.7012</v>
+      </c>
+    </row>
+    <row r="183" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B183" s="6">
+        <v>5</v>
+      </c>
+      <c r="C183" s="7">
+        <v>4</v>
+      </c>
+      <c r="D183" s="7">
+        <v>0</v>
+      </c>
+      <c r="E183" s="7">
+        <v>0.42608079999999998</v>
+      </c>
+      <c r="F183" s="7"/>
+      <c r="G183" s="8">
+        <f t="shared" si="19"/>
+        <v>400</v>
+      </c>
+      <c r="H183" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I183" s="8">
+        <f t="shared" si="21"/>
+        <v>42.608080000000001</v>
+      </c>
+    </row>
+    <row r="184" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B184" s="6">
+        <v>6</v>
+      </c>
+      <c r="C184" s="7">
+        <v>5</v>
+      </c>
+      <c r="D184" s="7">
+        <v>0</v>
+      </c>
+      <c r="E184" s="7">
+        <v>0.37820900000000002</v>
+      </c>
+      <c r="F184" s="7"/>
+      <c r="G184" s="8">
+        <f t="shared" si="19"/>
+        <v>500</v>
+      </c>
+      <c r="H184" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I184" s="8">
+        <f t="shared" si="21"/>
+        <v>37.820900000000002</v>
+      </c>
+    </row>
+    <row r="185" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B185" s="6">
+        <v>7</v>
+      </c>
+      <c r="C185" s="7">
+        <v>6</v>
+      </c>
+      <c r="D185" s="7">
+        <v>0</v>
+      </c>
+      <c r="E185" s="7">
+        <v>0.29702149999999999</v>
+      </c>
+      <c r="F185" s="7"/>
+      <c r="G185" s="8">
+        <f t="shared" si="19"/>
+        <v>600</v>
+      </c>
+      <c r="H185" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I185" s="8">
+        <f t="shared" si="21"/>
+        <v>29.70215</v>
+      </c>
+    </row>
+    <row r="186" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B186" s="6">
+        <v>8</v>
+      </c>
+      <c r="C186" s="7">
+        <v>7</v>
+      </c>
+      <c r="D186" s="7">
+        <v>1.2631086999999999E-2</v>
+      </c>
+      <c r="E186" s="7">
+        <v>0.24904570000000001</v>
+      </c>
+      <c r="F186" s="7"/>
+      <c r="G186" s="8">
+        <f t="shared" si="19"/>
+        <v>700</v>
+      </c>
+      <c r="H186" s="8">
+        <f t="shared" si="20"/>
+        <v>1.2631086999999999</v>
+      </c>
+      <c r="I186" s="8">
+        <f t="shared" si="21"/>
+        <v>24.90457</v>
+      </c>
+    </row>
+    <row r="187" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B187" s="6">
+        <v>9</v>
+      </c>
+      <c r="C187" s="7">
+        <v>8</v>
+      </c>
+      <c r="D187" s="7">
+        <v>1.5341377999999999E-2</v>
+      </c>
+      <c r="E187" s="7">
+        <v>0.42771789999999998</v>
+      </c>
+      <c r="F187" s="7"/>
+      <c r="G187" s="8">
+        <f t="shared" si="19"/>
+        <v>800</v>
+      </c>
+      <c r="H187" s="8">
+        <f t="shared" si="20"/>
+        <v>1.5341377999999999</v>
+      </c>
+      <c r="I187" s="8">
+        <f t="shared" si="21"/>
+        <v>42.771789999999996</v>
+      </c>
+    </row>
+    <row r="188" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B188" s="6">
+        <v>10</v>
+      </c>
+      <c r="C188" s="7">
+        <v>9</v>
+      </c>
+      <c r="D188" s="7">
+        <v>0</v>
+      </c>
+      <c r="E188" s="7">
+        <v>0.24475769999999999</v>
+      </c>
+      <c r="F188" s="7"/>
+      <c r="G188" s="8">
+        <f t="shared" si="19"/>
+        <v>900</v>
+      </c>
+      <c r="H188" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I188" s="8">
+        <f t="shared" si="21"/>
+        <v>24.475770000000001</v>
+      </c>
+    </row>
+    <row r="189" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B189" s="6">
+        <v>11</v>
+      </c>
+      <c r="C189" s="7">
+        <v>10</v>
+      </c>
+      <c r="D189" s="7">
+        <v>0</v>
+      </c>
+      <c r="E189" s="7">
+        <v>0.20388729999999999</v>
+      </c>
+      <c r="F189" s="7"/>
+      <c r="G189" s="8">
+        <f t="shared" si="19"/>
+        <v>1000</v>
+      </c>
+      <c r="H189" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I189" s="8">
+        <f t="shared" si="21"/>
+        <v>20.388729999999999</v>
+      </c>
+    </row>
+    <row r="190" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B190" s="6">
+        <v>12</v>
+      </c>
+      <c r="C190" s="7">
+        <v>11</v>
+      </c>
+      <c r="D190" s="7">
+        <v>0</v>
+      </c>
+      <c r="E190" s="7">
+        <v>0.3869264</v>
+      </c>
+      <c r="F190" s="7"/>
+      <c r="G190" s="8">
+        <f t="shared" si="19"/>
+        <v>1100</v>
+      </c>
+      <c r="H190" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I190" s="8">
+        <f t="shared" si="21"/>
+        <v>38.692639999999997</v>
+      </c>
+    </row>
+    <row r="191" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B191" s="6">
+        <v>13</v>
+      </c>
+      <c r="C191" s="7">
+        <v>12</v>
+      </c>
+      <c r="D191" s="7">
+        <v>0</v>
+      </c>
+      <c r="E191" s="7">
+        <v>0.43537550000000003</v>
+      </c>
+      <c r="F191" s="7"/>
+      <c r="G191" s="8">
+        <f t="shared" si="19"/>
+        <v>1200</v>
+      </c>
+      <c r="H191" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I191" s="8">
+        <f t="shared" si="21"/>
+        <v>43.537550000000003</v>
+      </c>
+    </row>
+    <row r="192" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B192" s="6">
+        <v>14</v>
+      </c>
+      <c r="C192" s="7">
+        <v>13</v>
+      </c>
+      <c r="D192" s="7">
+        <v>3.9321729999999997E-3</v>
+      </c>
+      <c r="E192" s="7">
+        <v>0.29307709999999998</v>
+      </c>
+      <c r="F192" s="7"/>
+      <c r="G192" s="8">
+        <f t="shared" si="19"/>
+        <v>1300</v>
+      </c>
+      <c r="H192" s="8">
+        <f t="shared" si="20"/>
+        <v>0.39321729999999999</v>
+      </c>
+      <c r="I192" s="8">
+        <f t="shared" si="21"/>
+        <v>29.307709999999997</v>
+      </c>
+    </row>
+    <row r="193" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B193" s="6">
+        <v>15</v>
+      </c>
+      <c r="C193" s="7">
+        <v>14</v>
+      </c>
+      <c r="D193" s="7">
+        <v>0</v>
+      </c>
+      <c r="E193" s="7">
+        <v>0.33883059999999998</v>
+      </c>
+      <c r="F193" s="7"/>
+      <c r="G193" s="8">
+        <f t="shared" si="19"/>
+        <v>1400</v>
+      </c>
+      <c r="H193" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I193" s="8">
+        <f t="shared" si="21"/>
+        <v>33.88306</v>
+      </c>
+    </row>
+    <row r="194" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B194" s="6">
+        <v>16</v>
+      </c>
+      <c r="C194" s="7">
+        <v>15</v>
+      </c>
+      <c r="D194" s="7">
+        <v>0</v>
+      </c>
+      <c r="E194" s="7">
+        <v>0.30422110000000002</v>
+      </c>
+      <c r="F194" s="7"/>
+      <c r="G194" s="8">
+        <f t="shared" si="19"/>
+        <v>1500</v>
+      </c>
+      <c r="H194" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I194" s="8">
+        <f t="shared" si="21"/>
+        <v>30.422110000000004</v>
+      </c>
+    </row>
+    <row r="195" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B195" s="6">
+        <v>17</v>
+      </c>
+      <c r="C195" s="7">
+        <v>16</v>
+      </c>
+      <c r="D195" s="7">
+        <v>0</v>
+      </c>
+      <c r="E195" s="7">
+        <v>0.32081799999999999</v>
+      </c>
+      <c r="F195" s="7"/>
+      <c r="G195" s="8">
+        <f t="shared" si="19"/>
+        <v>1600</v>
+      </c>
+      <c r="H195" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I195" s="8">
+        <f t="shared" si="21"/>
+        <v>32.081800000000001</v>
+      </c>
+    </row>
+    <row r="196" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B196" s="6">
+        <v>18</v>
+      </c>
+      <c r="C196" s="7">
+        <v>17</v>
+      </c>
+      <c r="D196" s="7">
+        <v>0</v>
+      </c>
+      <c r="E196" s="7">
+        <v>0.4499129</v>
+      </c>
+      <c r="F196" s="7"/>
+      <c r="G196" s="8">
+        <f t="shared" si="19"/>
+        <v>1700</v>
+      </c>
+      <c r="H196" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I196" s="8">
+        <f t="shared" si="21"/>
+        <v>44.991289999999999</v>
+      </c>
+    </row>
+    <row r="197" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B197" s="6">
+        <v>19</v>
+      </c>
+      <c r="C197" s="7">
+        <v>18</v>
+      </c>
+      <c r="D197" s="7">
+        <v>0</v>
+      </c>
+      <c r="E197" s="7">
+        <v>0.21458720000000001</v>
+      </c>
+      <c r="F197" s="7"/>
+      <c r="G197" s="8">
+        <f t="shared" si="19"/>
+        <v>1800</v>
+      </c>
+      <c r="H197" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I197" s="8">
+        <f t="shared" si="21"/>
+        <v>21.45872</v>
+      </c>
+    </row>
+    <row r="198" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B198" s="6">
+        <v>20</v>
+      </c>
+      <c r="C198" s="7">
+        <v>19</v>
+      </c>
+      <c r="D198" s="7">
+        <v>0</v>
+      </c>
+      <c r="E198" s="7">
+        <v>0.2227181</v>
+      </c>
+      <c r="F198" s="7"/>
+      <c r="G198" s="8">
+        <f t="shared" si="19"/>
+        <v>1900</v>
+      </c>
+      <c r="H198" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I198" s="8">
+        <f t="shared" si="21"/>
+        <v>22.271809999999999</v>
+      </c>
+    </row>
+    <row r="199" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B199" s="6">
+        <v>21</v>
+      </c>
+      <c r="C199" s="7">
+        <v>20</v>
+      </c>
+      <c r="D199" s="7">
+        <v>7.5435770000000001E-3</v>
+      </c>
+      <c r="E199" s="7">
+        <v>0.34424589999999999</v>
+      </c>
+      <c r="F199" s="7"/>
+      <c r="G199" s="8">
+        <f t="shared" si="19"/>
+        <v>2000</v>
+      </c>
+      <c r="H199" s="8">
+        <f t="shared" si="20"/>
+        <v>0.75435770000000002</v>
+      </c>
+      <c r="I199" s="8">
+        <f t="shared" si="21"/>
+        <v>34.424590000000002</v>
+      </c>
+    </row>
+    <row r="200" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B200" s="6">
+        <v>22</v>
+      </c>
+      <c r="C200" s="7">
+        <v>21</v>
+      </c>
+      <c r="D200" s="7">
+        <v>0</v>
+      </c>
+      <c r="E200" s="7">
+        <v>0.16467019999999999</v>
+      </c>
+      <c r="F200" s="7"/>
+      <c r="G200" s="8">
+        <f t="shared" si="19"/>
+        <v>2100</v>
+      </c>
+      <c r="H200" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I200" s="8">
+        <f t="shared" si="21"/>
+        <v>16.467019999999998</v>
+      </c>
+    </row>
+    <row r="201" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B201" s="6">
+        <v>23</v>
+      </c>
+      <c r="C201" s="7">
+        <v>22</v>
+      </c>
+      <c r="D201" s="7">
+        <v>1.139944E-2</v>
+      </c>
+      <c r="E201" s="7">
+        <v>0.20116999999999999</v>
+      </c>
+      <c r="F201" s="7"/>
+      <c r="G201" s="8">
+        <f t="shared" si="19"/>
+        <v>2200</v>
+      </c>
+      <c r="H201" s="8">
+        <f t="shared" si="20"/>
+        <v>1.1399440000000001</v>
+      </c>
+      <c r="I201" s="8">
+        <f t="shared" si="21"/>
+        <v>20.116999999999997</v>
+      </c>
+    </row>
+    <row r="202" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B202" s="6">
+        <v>24</v>
+      </c>
+      <c r="C202" s="7">
+        <v>23</v>
+      </c>
+      <c r="D202" s="7">
+        <v>2.7911569999999998E-3</v>
+      </c>
+      <c r="E202" s="7">
+        <v>0.1514673</v>
+      </c>
+      <c r="F202" s="7"/>
+      <c r="G202" s="8">
+        <f t="shared" si="19"/>
+        <v>2300</v>
+      </c>
+      <c r="H202" s="8">
+        <f t="shared" si="20"/>
+        <v>0.27911569999999997</v>
+      </c>
+      <c r="I202" s="8">
+        <f t="shared" si="21"/>
+        <v>15.14673</v>
+      </c>
+    </row>
+    <row r="203" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B203" s="6">
+        <v>25</v>
+      </c>
+      <c r="C203" s="7">
+        <v>24</v>
+      </c>
+      <c r="D203" s="7">
+        <v>0</v>
+      </c>
+      <c r="E203" s="7">
+        <v>0.36809609999999998</v>
+      </c>
+      <c r="F203" s="7"/>
+      <c r="G203" s="8">
+        <f t="shared" si="19"/>
+        <v>2400</v>
+      </c>
+      <c r="H203" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I203" s="8">
+        <f t="shared" si="21"/>
+        <v>36.809609999999999</v>
+      </c>
+    </row>
+    <row r="204" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B204" s="6">
+        <v>26</v>
+      </c>
+      <c r="C204" s="7">
+        <v>25</v>
+      </c>
+      <c r="D204" s="7">
+        <v>0</v>
+      </c>
+      <c r="E204" s="7">
+        <v>0.22212409999999999</v>
+      </c>
+      <c r="F204" s="7"/>
+      <c r="G204" s="8">
+        <f t="shared" si="19"/>
+        <v>2500</v>
+      </c>
+      <c r="H204" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I204" s="8">
+        <f t="shared" si="21"/>
+        <v>22.212409999999998</v>
+      </c>
+    </row>
+    <row r="205" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B205" s="6">
+        <v>27</v>
+      </c>
+      <c r="C205" s="7">
+        <v>26</v>
+      </c>
+      <c r="D205" s="7">
+        <v>0</v>
+      </c>
+      <c r="E205" s="7">
+        <v>0.33013429999999999</v>
+      </c>
+      <c r="F205" s="7"/>
+      <c r="G205" s="8">
+        <f t="shared" si="19"/>
+        <v>2600</v>
+      </c>
+      <c r="H205" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I205" s="8">
+        <f t="shared" si="21"/>
+        <v>33.01343</v>
+      </c>
+    </row>
+    <row r="206" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B206" s="6">
+        <v>28</v>
+      </c>
+      <c r="C206" s="7">
+        <v>27</v>
+      </c>
+      <c r="D206" s="7">
+        <v>0</v>
+      </c>
+      <c r="E206" s="7">
+        <v>0.46641159999999998</v>
+      </c>
+      <c r="F206" s="7"/>
+      <c r="G206" s="8">
+        <f t="shared" si="19"/>
+        <v>2700</v>
+      </c>
+      <c r="H206" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I206" s="8">
+        <f t="shared" si="21"/>
+        <v>46.641159999999999</v>
+      </c>
+    </row>
+    <row r="207" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B207" s="6">
+        <v>29</v>
+      </c>
+      <c r="C207" s="7">
+        <v>28</v>
+      </c>
+      <c r="D207" s="7">
+        <v>0</v>
+      </c>
+      <c r="E207" s="7">
+        <v>0.46146890000000002</v>
+      </c>
+      <c r="F207" s="7"/>
+      <c r="G207" s="8">
+        <f t="shared" si="19"/>
+        <v>2800</v>
+      </c>
+      <c r="H207" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I207" s="8">
+        <f t="shared" si="21"/>
+        <v>46.146889999999999</v>
+      </c>
+    </row>
+    <row r="208" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B208" s="6">
+        <v>30</v>
+      </c>
+      <c r="C208" s="7">
+        <v>29</v>
+      </c>
+      <c r="D208" s="7">
+        <v>0</v>
+      </c>
+      <c r="E208" s="7">
+        <v>0.23624390000000001</v>
+      </c>
+      <c r="F208" s="7"/>
+      <c r="G208" s="8">
+        <f t="shared" si="19"/>
+        <v>2900</v>
+      </c>
+      <c r="H208" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I208" s="8">
+        <f t="shared" si="21"/>
+        <v>23.624390000000002</v>
+      </c>
+    </row>
+    <row r="209" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B209" s="6">
+        <v>31</v>
+      </c>
+      <c r="C209" s="7">
+        <v>30</v>
+      </c>
+      <c r="D209" s="7">
+        <v>0</v>
+      </c>
+      <c r="E209" s="7">
+        <v>0.23048350000000001</v>
+      </c>
+      <c r="F209" s="7"/>
+      <c r="G209" s="8">
+        <f t="shared" si="19"/>
+        <v>3000</v>
+      </c>
+      <c r="H209" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I209" s="8">
+        <f t="shared" si="21"/>
+        <v>23.048349999999999</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>